<commit_message>
Last set of edits from TS.
</commit_message>
<xml_diff>
--- a/assets/new-COVID-primer-set-stats.xlsx
+++ b/assets/new-COVID-primer-set-stats.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="138">
   <si>
-    <t xml:space="preserve"># Designed by Tomer Altman. Licensed as Creative Commons Attribution 4.0 International 4.0 (CC BY 4.0) https://creativecommons.org/licenses/by/4.0/</t>
+    <t xml:space="preserve"># Designed by Tomer Altman. Licensed as Creative Commons Attribution 4.0 International (CC BY 4.0) https://creativecommons.org/licenses/by/4.0/</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -532,7 +532,7 @@
   <dimension ref="A1:V56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>